<commit_message>
went through the whole code, added comments and removed minor bugs
</commit_message>
<xml_diff>
--- a/Test_Input_Single.xlsx
+++ b/Test_Input_Single.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20379"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7CF2FEF-D9CD-4052-A9B2-51C72FFFB681}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5EC13C3-F8BF-49C5-96A9-F4A649772AE9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -659,37 +659,37 @@
   <dimension ref="A1:AI7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.1328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.86328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.3984375" customWidth="1"/>
-    <col min="9" max="9" width="11.86328125" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" customWidth="1"/>
     <col min="12" max="12" width="14" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.59765625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.3984375" customWidth="1"/>
-    <col min="15" max="15" width="22.59765625" customWidth="1"/>
-    <col min="16" max="16" width="15.1328125" customWidth="1"/>
-    <col min="17" max="17" width="11.265625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.86328125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.265625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.1328125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.73046875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.265625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.73046875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.42578125" customWidth="1"/>
+    <col min="15" max="15" width="22.5703125" customWidth="1"/>
+    <col min="16" max="16" width="15.140625" customWidth="1"/>
+    <col min="17" max="17" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="17" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="16.59765625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="19.59765625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="24.73046875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="17" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="14.3984375" customWidth="1"/>
+    <col min="32" max="32" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -790,7 +790,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>33</v>
       </c>
@@ -834,7 +834,7 @@
         <v>29</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="P2" s="4" t="s">
         <v>31</v>
@@ -893,7 +893,7 @@
       <c r="AH2" s="4"/>
       <c r="AI2" s="4"/>
     </row>
-    <row r="3" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>40</v>
       </c>
@@ -934,13 +934,13 @@
         <v>4300</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
       <c r="B6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="6" t="s">
         <v>55</v>
@@ -991,17 +991,17 @@
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.59765625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.86328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="24" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.3984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1039,7 +1039,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>40</v>
       </c>
@@ -1071,13 +1071,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
       <c r="B7" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="12"/>
       <c r="B8" s="6" t="s">
         <v>63</v>

</xml_diff>